<commit_message>
fix: solucion o cambio
</commit_message>
<xml_diff>
--- a/data/Plan Personalizado de actividades SSO 2026 - Alioska Saavedra.xlsx
+++ b/data/Plan Personalizado de actividades SSO 2026 - Alioska Saavedra.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JOACO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JoacoScope\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11002246-342D-4A88-AA03-43FAC423F73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4482CB-2D55-4CF6-B69A-6134C9333531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Plan personalizado de prevención de riesgos</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Inspeccion de seguridad</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -2036,7 +2039,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScaleSheetLayoutView="180" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -2179,11 +2182,11 @@
         <v>3</v>
       </c>
       <c r="F9" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <f>F9/E9</f>
-        <v>1</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H9" s="22" t="s">
         <v>25</v>
@@ -2202,11 +2205,11 @@
         <v>2</v>
       </c>
       <c r="F10" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="6">
         <f t="shared" ref="G10:G12" si="0">F10/E10</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="24" t="s">
         <v>23</v>
@@ -2349,8 +2352,8 @@
       <c r="D18" s="40"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
-      <c r="G18" s="36">
-        <v>1</v>
+      <c r="G18" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="H18" s="16" t="s">
         <v>33</v>
@@ -2382,9 +2385,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="106" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <ignoredErrors>
-    <ignoredError sqref="G17" numberStoredAsText="1"/>
-  </ignoredErrors>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>